<commit_message>
Added compiled annual data to monthly data spreadsheets in edmc/new
</commit_message>
<xml_diff>
--- a/edmc_databank/new/elecgenofelecutils-monthly.xlsx
+++ b/edmc_databank/new/elecgenofelecutils-monthly.xlsx
@@ -1,20 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\achubbz\Documents\GitHub\i2cner\edmc_databank\new\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F3890B-B629-4DDA-A29E-DABC62054A45}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="660" windowWidth="27555" windowHeight="11985"/>
+    <workbookView xWindow="840" yWindow="660" windowWidth="27552" windowHeight="11988" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>Electricity generation of electricity utilities</t>
   </si>
@@ -29,9 +36,6 @@
   </si>
   <si>
     <t xml:space="preserve">Unit: </t>
-  </si>
-  <si>
-    <t>1000KWH</t>
   </si>
   <si>
     <t>Total</t>
@@ -117,15 +121,27 @@
   <si>
     <t>With the enforcement of the 2nd Amendment Electricity Business Act, the contents of the power Research and Statistics has changed significantly from the 2016 April .</t>
   </si>
+  <si>
+    <t>MWh</t>
+  </si>
+  <si>
+    <t>FY</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>TWh</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="176" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="177" formatCode="mm/yyyy"/>
-    <numFmt numFmtId="178" formatCode="#,##0.00_ "/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="165" formatCode="mm/yyyy"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00_ "/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -181,20 +197,20 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
@@ -203,21 +219,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
-    <cellStyle name="標準" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -259,7 +286,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -291,9 +318,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -325,6 +370,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -500,27 +563,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q384"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="10" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="10" topLeftCell="B357" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A360" sqref="A360"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
-    <col min="2" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.6640625" customWidth="1"/>
+    <col min="2" max="7" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -528,7 +591,7 @@
         <v>0</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -552,57 +615,57 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" s="3" customFormat="1" ht="55.2">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" s="3" customFormat="1" ht="51">
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="K6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="O6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="P6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="Q6" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:17" s="3" customFormat="1" hidden="1"/>
@@ -13347,39 +13410,245 @@
     </row>
     <row r="379" spans="1:17">
       <c r="A379" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="380" spans="1:17">
       <c r="A380" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="381" spans="1:17">
       <c r="A381" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="382" spans="1:17">
       <c r="A382" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="383" spans="1:17">
       <c r="A383" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="384" spans="1:17">
       <c r="A384" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="F1" location="Sheet1!A379" display="To notes"/>
+    <hyperlink ref="F1" location="Sheet1!A379" display="To notes" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{574E408C-6C80-4599-930A-3EDD6342366B}">
+  <dimension ref="A1:N6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="1" max="1" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="14" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="69">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B2">
+        <v>68.563820000000007</v>
+      </c>
+      <c r="C2">
+        <v>234.514005</v>
+      </c>
+      <c r="D2">
+        <v>399.27104200000002</v>
+      </c>
+      <c r="E2">
+        <v>108.13489</v>
+      </c>
+      <c r="F2">
+        <v>0.44575799999999999</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0.75228700000000004</v>
+      </c>
+      <c r="I2">
+        <v>1.8842319999999999</v>
+      </c>
+      <c r="J2">
+        <v>0.236849</v>
+      </c>
+      <c r="K2">
+        <v>9.3027499999999996</v>
+      </c>
+      <c r="L2">
+        <v>0.16267200000000001</v>
+      </c>
+      <c r="M2">
+        <v>8.5568000000000005E-2</v>
+      </c>
+      <c r="N2">
+        <v>2.435616</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B3">
+        <v>70.254693000000003</v>
+      </c>
+      <c r="C3">
+        <v>231.421055</v>
+      </c>
+      <c r="D3">
+        <v>411.91667999999999</v>
+      </c>
+      <c r="E3">
+        <v>72.570868000000004</v>
+      </c>
+      <c r="F3">
+        <v>0.35130400000000001</v>
+      </c>
+      <c r="G3">
+        <v>0.78613500000000003</v>
+      </c>
+      <c r="H3">
+        <v>0.71792599999999995</v>
+      </c>
+      <c r="I3">
+        <v>1.972288</v>
+      </c>
+      <c r="J3">
+        <v>0.233207</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>3.4347999999999997E-2</v>
+      </c>
+      <c r="M3">
+        <v>8.8941000000000006E-2</v>
+      </c>
+      <c r="N3">
+        <v>2.418946</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B4">
+        <v>74.800523999999996</v>
+      </c>
+      <c r="C4">
+        <v>232.61803599999999</v>
+      </c>
+      <c r="D4">
+        <v>383.29288500000001</v>
+      </c>
+      <c r="E4">
+        <v>57.693227</v>
+      </c>
+      <c r="F4">
+        <v>0.43100500000000003</v>
+      </c>
+      <c r="G4">
+        <v>0.91400199999999998</v>
+      </c>
+      <c r="H4">
+        <v>0.70991099999999996</v>
+      </c>
+      <c r="I4">
+        <v>2.0061719999999998</v>
+      </c>
+      <c r="J4">
+        <v>0.22406999999999999</v>
+      </c>
+      <c r="K4">
+        <v>9.4372849999999993</v>
+      </c>
+      <c r="L4">
+        <v>6.7165000000000002E-2</v>
+      </c>
+      <c r="M4">
+        <v>9.8534999999999998E-2</v>
+      </c>
+      <c r="N4">
+        <v>2.3841030000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>